<commit_message>
Changed L1 inductor from 1uH to 1.5uH for higher output current stability. Generated PDF schematics. Updated BoM file.
</commit_message>
<xml_diff>
--- a/cam/DCDC-12V5V1A_2023-06-18-BoM.xlsx
+++ b/cam/DCDC-12V5V1A_2023-06-18-BoM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DC-DC\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65147045-1049-4C81-8677-5CE6173F80CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD71911-E5CD-4103-B017-D61F77D0BCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="3156" windowWidth="26388" windowHeight="20412" xr2:uid="{F7F56201-6554-4440-82E7-3E6343A878DA}"/>
+    <workbookView xWindow="1428" yWindow="3504" windowWidth="26388" windowHeight="20412" xr2:uid="{F7F56201-6554-4440-82E7-3E6343A878DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>1uH</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>C23219</t>
   </si>
   <si>
-    <t>C354578</t>
-  </si>
-  <si>
     <t>SMD</t>
   </si>
   <si>
@@ -226,6 +220,12 @@
   </si>
   <si>
     <t>C72043</t>
+  </si>
+  <si>
+    <t>1.5uH</t>
+  </si>
+  <si>
+    <t>C354573</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,16 +613,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -636,13 +636,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -656,13 +656,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -676,13 +676,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -696,13 +696,13 @@
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -716,13 +716,13 @@
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -733,19 +733,19 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -753,16 +753,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>
@@ -773,16 +773,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -793,16 +793,16 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
@@ -813,16 +813,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
@@ -833,19 +833,19 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
         <v>26</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -853,19 +853,19 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>